<commit_message>
changes for package release
</commit_message>
<xml_diff>
--- a/Documents/Config/Live_Config.xlsx
+++ b/Documents/Config/Live_Config.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\GFD218DF\x953922$\UiPath\rpa-future-farming-cross-compliance\Documents\Config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\GFD218DF\x952359$\Development\rpa-future-farming-cross-compliance\Documents\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EF0DECC-5827-4095-B7F7-F6FDD6D55335}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -153,9 +152,6 @@
     <t>Path for ARF Matched Folder where SBI folders containing a matching ARF and CRF are placed for Master Copy.</t>
   </si>
   <si>
-    <t xml:space="preserve">https://rpa-csc-uat.crm4.dynamics.com/main.aspx                                                        </t>
-  </si>
-  <si>
     <t>Timeouts</t>
   </si>
   <si>
@@ -240,15 +236,6 @@
     <t>CiiMailbox</t>
   </si>
   <si>
-    <t>SAGReports.XC@rpa.gov.uk</t>
-  </si>
-  <si>
-    <t>XCAnimalHealthStandaloneandselected@rpa.gov.uk</t>
-  </si>
-  <si>
-    <t>XCRPAreports@rpa.gov.uk</t>
-  </si>
-  <si>
     <t>CrossCompliance.DiscrepancyReports@rpa.gov.uk</t>
   </si>
   <si>
@@ -354,9 +341,6 @@
     <t>XcomUrl</t>
   </si>
   <si>
-    <t>http://rpa-domino-dev.dev.azure.defra.cloud/intranet/xcompliance2015.nsf</t>
-  </si>
-  <si>
     <t>Url for Xcom test</t>
   </si>
   <si>
@@ -391,12 +375,27 @@
   </si>
   <si>
     <t>ready to be receipted for all crf types - use for deployment 1 only</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://rpa-csc-prod.crm4.dynamics.com/main.aspx                                                        </t>
+  </si>
+  <si>
+    <t>http://crosscompliancedatabase/intranet/xcompliance2015.nsf/</t>
+  </si>
+  <si>
+    <t>SM-RPA-XC SAG Reports</t>
+  </si>
+  <si>
+    <t>SM-RPA-XCRPAreports</t>
+  </si>
+  <si>
+    <t>SM-RPA-XC Animal Health Stand alone and selected</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -520,12 +519,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C55" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="A1:C55" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C55" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A1:C55"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Value" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Description" dataDxfId="0"/>
+    <tableColumn id="1" name="Name" dataDxfId="2"/>
+    <tableColumn id="2" name="Value" dataDxfId="1"/>
+    <tableColumn id="3" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -827,11 +826,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -862,107 +861,107 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B5" s="7" t="b">
         <v>1</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B6" s="7" t="b">
         <v>1</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B7" s="7" t="b">
         <v>1</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B8" s="7" t="b">
         <v>1</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B9" s="7" t="b">
         <v>1</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B10" s="7" t="b">
         <v>1</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B11" s="7" t="b">
         <v>1</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B13" s="4">
         <v>3</v>
@@ -971,68 +970,68 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B14" s="4">
         <v>1000</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B15" s="4">
         <v>3000</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B16" s="4">
         <v>5000</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B17" s="4">
         <v>30000</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B18" s="4">
         <v>60000</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B19" s="4">
         <v>120000</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1047,7 +1046,7 @@
         <v>31</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>42</v>
+        <v>117</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>32</v>
@@ -1055,46 +1054,46 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="B24" s="8" t="s">
-        <v>63</v>
-      </c>
       <c r="C24" s="7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -1227,80 +1226,80 @@
     </row>
     <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C40" s="4" t="s">
         <v>116</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>71</v>
+        <v>119</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>72</v>
+        <v>121</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B44" s="4" t="s">
         <v>70</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -1310,66 +1309,66 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed deployment issues, Resolve Case done, Attaching docs started
</commit_message>
<xml_diff>
--- a/Documents/Config/Live_Config.xlsx
+++ b/Documents/Config/Live_Config.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\GFD218DF\x952359$\Development\rpa-future-farming-cross-compliance\Documents\Config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\GFD218DF\x953922$\UiPath\rpa-future-farming-cross-compliance\Documents\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E89DFB4-44A1-4A45-A64B-632DAF4EFFFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="125">
   <si>
     <t>Name</t>
   </si>
@@ -390,12 +391,21 @@
   </si>
   <si>
     <t>SM-RPA-XC Animal Health Stand alone and selected</t>
+  </si>
+  <si>
+    <t>CRMInfo</t>
+  </si>
+  <si>
+    <t>DocumentType</t>
+  </si>
+  <si>
+    <t>LTRCUST</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -519,12 +529,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C55" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="A1:C55"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C57" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A1:C57" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Name" dataDxfId="2"/>
-    <tableColumn id="2" name="Value" dataDxfId="1"/>
-    <tableColumn id="3" name="Description" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Value" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -826,11 +836,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C55"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1304,70 +1314,83 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="6" t="s">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B50" s="4" t="s">
         <v>89</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="B57" s="4" t="s">
         <v>98</v>
       </c>
     </row>

</xml_diff>